<commit_message>
make changes to create to_list method and update code in add_item, remove_item, search_item make changes to print return message when called while adding
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\putta\PycharmProjects\pythonProject2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F98121-545C-4A5C-B440-B0A05EDCF9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BC2082-AA56-4C37-B20C-33F3FEFE1CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3246,13 +3246,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3557,19 +3556,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J660"/>
+  <dimension ref="A1:F660"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A642" workbookViewId="0">
+      <selection activeCell="P648" sqref="P648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3589,7 +3584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3609,7 +3604,7 @@
         <v>44240.647800925923</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3629,7 +3624,7 @@
         <v>44950.577599999997</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3648,9 +3643,8 @@
       <c r="F4" s="2">
         <v>44831.569900000002</v>
       </c>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3670,7 +3664,7 @@
         <v>44316.348400000003</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3690,7 +3684,7 @@
         <v>44820.612800000003</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3710,7 +3704,7 @@
         <v>44316.559099999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3730,7 +3724,7 @@
         <v>44427.335099999997</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3750,7 +3744,7 @@
         <v>45008.464999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3770,7 +3764,7 @@
         <v>44197.512999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -3790,7 +3784,7 @@
         <v>45190.4735</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -3810,7 +3804,7 @@
         <v>44709.631300000001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3830,7 +3824,7 @@
         <v>44286.679199999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -3850,7 +3844,7 @@
         <v>45055.519099999998</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -3870,7 +3864,7 @@
         <v>44722.395100000002</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
make changes to add_method and add bulk input method
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\putta\PycharmProjects\pythonProject2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BC2082-AA56-4C37-B20C-33F3FEFE1CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32EF49C-75B7-4534-80E7-8AEE81AC4C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3558,8 +3558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F660"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A642" workbookViewId="0">
-      <selection activeCell="P648" sqref="P648"/>
+    <sheetView tabSelected="1" topLeftCell="A641" workbookViewId="0">
+      <selection activeCell="A661" sqref="A661:F661"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added comments and docstrings along with requirements file
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\putta\PycharmProjects\pythonProject2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32EF49C-75B7-4534-80E7-8AEE81AC4C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BD0A2B-AC14-4BB7-AB4A-386DAED2DE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3558,8 +3558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F660"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A641" workbookViewId="0">
-      <selection activeCell="A661" sqref="A661:F661"/>
+    <sheetView tabSelected="1" topLeftCell="A642" workbookViewId="0">
+      <selection activeCell="J658" sqref="J658"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
removed excel test data
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\putta\PycharmProjects\pythonProject2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44886E48-AE09-4E3B-BED5-46DA5358AA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BEA038-35B5-46EA-8547-B1AB53BE27B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3565,7 +3565,7 @@
   <dimension ref="A1:F661"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>